<commit_message>
load data fixes to the comments.md
</commit_message>
<xml_diff>
--- a/assets/teamstats.xlsx
+++ b/assets/teamstats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\apex_textdemo\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4CE7C0F-EE80-412E-8CBA-D57FEAE28F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2131DDF-2E65-4A8D-8160-F36846DE1C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -104,15 +104,6 @@
   </si>
   <si>
     <t>PS</t>
-  </si>
-  <si>
-    <t>AVG</t>
-  </si>
-  <si>
-    <t>OBP</t>
-  </si>
-  <si>
-    <t>SLG</t>
   </si>
   <si>
     <t>VIDEO</t>
@@ -251,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="sheet1" displayName="sheet1" ref="A1:AF13" totalsRowShown="0">
-  <tableColumns count="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="sheet1" displayName="sheet1" ref="A1:AC13" totalsRowShown="0">
+  <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="JERSEY"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NAME"/>
@@ -281,9 +272,6 @@
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="XBH"/>
     <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="TB"/>
     <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="PS"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="AVG"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="OBP"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="SLG"/>
     <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="VIDEO"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="1" showLastColumn="1" showRowStripes="0" showColumnStripes="0"/>
@@ -587,11 +575,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,11 +601,10 @@
     <col min="25" max="26" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,20 +689,11 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="2" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -723,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3">
         <v>20</v>
@@ -800,18 +778,9 @@
       <c r="AB2" s="3">
         <v>198</v>
       </c>
-      <c r="AC2" s="3">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="AF2" s="4"/>
+      <c r="AC2" s="4"/>
     </row>
-    <row r="3" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -819,7 +788,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3">
         <v>14</v>
@@ -896,18 +865,9 @@
       <c r="AB3" s="3">
         <v>159</v>
       </c>
-      <c r="AC3" s="3">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>0.441</v>
-      </c>
-      <c r="AE3" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="AF3" s="4"/>
+      <c r="AC3" s="4"/>
     </row>
-    <row r="4" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -915,7 +875,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3">
         <v>20</v>
@@ -992,18 +952,9 @@
       <c r="AB4" s="3">
         <v>225</v>
       </c>
-      <c r="AC4" s="3">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>0.55700000000000005</v>
-      </c>
-      <c r="AE4" s="3">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="AF4" s="4"/>
+      <c r="AC4" s="4"/>
     </row>
-    <row r="5" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1011,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3">
         <v>20</v>
@@ -1088,18 +1039,9 @@
       <c r="AB5" s="3">
         <v>231</v>
       </c>
-      <c r="AC5" s="3">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="AE5" s="3">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="AF5" s="4"/>
+      <c r="AC5" s="4"/>
     </row>
-    <row r="6" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1107,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3">
         <v>18</v>
@@ -1184,20 +1126,11 @@
       <c r="AB6" s="3">
         <v>178</v>
       </c>
-      <c r="AC6" s="3">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="AD6" s="3">
-        <v>0.46300000000000002</v>
-      </c>
-      <c r="AE6" s="3">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="AF6" s="4" t="s">
-        <v>37</v>
+      <c r="AC6" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1205,7 +1138,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3">
         <v>14</v>
@@ -1282,18 +1215,9 @@
       <c r="AB7" s="3">
         <v>113</v>
       </c>
-      <c r="AC7" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="AE7" s="3">
-        <v>0.36</v>
-      </c>
-      <c r="AF7" s="4"/>
+      <c r="AC7" s="4"/>
     </row>
-    <row r="8" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1301,7 +1225,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D8" s="3">
         <v>20</v>
@@ -1378,18 +1302,9 @@
       <c r="AB8" s="3">
         <v>180</v>
       </c>
-      <c r="AC8" s="3">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="AD8" s="3">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="AE8" s="3">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="AF8" s="4"/>
+      <c r="AC8" s="4"/>
     </row>
-    <row r="9" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1397,7 +1312,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3">
         <v>20</v>
@@ -1474,18 +1389,9 @@
       <c r="AB9" s="3">
         <v>187</v>
       </c>
-      <c r="AC9" s="3">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="AD9" s="3">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="AE9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="AF9" s="4"/>
+      <c r="AC9" s="4"/>
     </row>
-    <row r="10" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1493,7 +1399,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10" s="3">
         <v>20</v>
@@ -1570,18 +1476,9 @@
       <c r="AB10" s="3">
         <v>205</v>
       </c>
-      <c r="AC10" s="3">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="AD10" s="3">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="AE10" s="3">
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="AF10" s="4"/>
+      <c r="AC10" s="4"/>
     </row>
-    <row r="11" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1589,7 +1486,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3">
         <v>19</v>
@@ -1666,18 +1563,9 @@
       <c r="AB11" s="3">
         <v>189</v>
       </c>
-      <c r="AC11" s="3">
-        <v>0.188</v>
-      </c>
-      <c r="AD11" s="3">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="AE11" s="3">
-        <v>0.219</v>
-      </c>
-      <c r="AF11" s="4"/>
+      <c r="AC11" s="4"/>
     </row>
-    <row r="12" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1685,7 +1573,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="3">
         <v>18</v>
@@ -1762,18 +1650,9 @@
       <c r="AB12" s="3">
         <v>155</v>
       </c>
-      <c r="AC12" s="3">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="AD12" s="3">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="AE12" s="3">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="AF12" s="4"/>
+      <c r="AC12" s="4"/>
     </row>
-    <row r="13" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1781,7 +1660,7 @@
         <v>99</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3">
         <v>20</v>
@@ -1858,16 +1737,7 @@
       <c r="AB13" s="3">
         <v>194</v>
       </c>
-      <c r="AC13" s="3">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="AD13" s="3">
-        <v>0.46200000000000002</v>
-      </c>
-      <c r="AE13" s="3">
-        <v>0.27</v>
-      </c>
-      <c r="AF13" s="4"/>
+      <c r="AC13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>